<commit_message>
New changes for summary
</commit_message>
<xml_diff>
--- a/OldMutual/Output/StatementSummary.xlsx
+++ b/OldMutual/Output/StatementSummary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vishn\OneDrive\Desktop\TechniX_Projects\UAP_OldMutual_Reconciliation_Process\old-mutual\OldMutual\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC021576-C49A-4321-8232-3602053DCBA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{833BFA1A-7081-4646-B54E-C53294A438F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25740" yWindow="3675" windowWidth="17280" windowHeight="8880" xr2:uid="{945A756C-64EB-4F47-AC63-805CC3E96EF8}"/>
+    <workbookView xWindow="3036" yWindow="3036" windowWidth="17280" windowHeight="8880" xr2:uid="{14F1490D-BA2D-4F34-9C48-3F11AB17B7E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -492,7 +492,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6381D52B-57C5-4C75-88A6-E58959BFF0F1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4938E3E8-DC99-4915-AED0-214590074476}">
   <dimension ref="D10:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -521,7 +521,7 @@
         <v>5</v>
       </c>
       <c r="G11">
-        <v>3006773320</v>
+        <v>2481217.77</v>
       </c>
       <c r="H11" t="s">
         <v>6</v>
@@ -665,7 +665,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EAD202D-5A6C-48D6-B4D5-FFD692480E67}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A80645-0EA3-4A62-8D5A-1E390A34C55E}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>